<commit_message>
All files from all projects
</commit_message>
<xml_diff>
--- a/Python/Optimal Power Flow with MINLP/IEEE30.xlsx
+++ b/Python/Optimal Power Flow with MINLP/IEEE30.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Desktop\Crecimiento Personal\Python\OPF Pyomo\Optimal-Power-Flow-in-python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo Trabajo\Desktop\My Github Repos\Portfolio\Python\Optimal Power Flow with MINLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A415A1-3E62-433F-9051-97AAA698C7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEE4564-6EE0-4215-A12B-AB4BBC443628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BUS" sheetId="1" r:id="rId1"/>
     <sheet name="RAMAS" sheetId="3" r:id="rId2"/>
     <sheet name="GEN" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -102,8 +113,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -193,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -225,6 +238,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,13 +527,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -539,9 +559,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="8">
         <v>1</v>
@@ -558,16 +578,16 @@
       <c r="F2" s="7">
         <v>0</v>
       </c>
-      <c r="G2" s="7">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="16">
+        <v>0</v>
+      </c>
+      <c r="H2" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="8">
         <v>2</v>
@@ -584,719 +604,719 @@
       <c r="F3" s="7">
         <v>0</v>
       </c>
-      <c r="G3" s="7">
-        <v>21.7</v>
-      </c>
-      <c r="H3" s="7">
-        <v>12.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="16">
+        <v>0.217</v>
+      </c>
+      <c r="H3" s="16">
+        <v>0.127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="16">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H4" s="16">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0</v>
-      </c>
-      <c r="G4" s="7">
-        <v>2.4</v>
-      </c>
-      <c r="H4" s="7">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="16">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="H5" s="16">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="10">
-        <v>0</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0</v>
-      </c>
-      <c r="G5" s="9">
-        <v>7.6</v>
-      </c>
-      <c r="H5" s="9">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="10">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0</v>
-      </c>
-      <c r="G6" s="9">
-        <v>94.2</v>
-      </c>
-      <c r="H6" s="9">
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="16">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="H8" s="16">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="H9" s="16">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0</v>
+      </c>
+      <c r="H10" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="16">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+      <c r="G12" s="16">
+        <v>0</v>
+      </c>
+      <c r="H12" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="16">
+        <v>0.112</v>
+      </c>
+      <c r="H13" s="16">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="16">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H15" s="16">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="16">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="H16" s="16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H17" s="16">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="11">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0</v>
+      </c>
+      <c r="G18" s="17">
+        <v>0.09</v>
+      </c>
+      <c r="H18" s="17">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
+        <v>17</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="17">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H19" s="17">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="11">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0</v>
+      </c>
+      <c r="G20" s="17">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="H20" s="17">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10">
-        <v>0</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="9">
-        <v>0</v>
-      </c>
-      <c r="H7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>7</v>
-      </c>
-      <c r="B8" s="10">
-        <v>0</v>
-      </c>
-      <c r="C8" s="7">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7">
-        <v>0</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9">
-        <v>22.8</v>
-      </c>
-      <c r="H8" s="9">
-        <v>10.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="7">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
-        <v>30</v>
-      </c>
-      <c r="H9" s="9">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="7">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7">
-        <v>0</v>
-      </c>
-      <c r="G10" s="9">
-        <v>0</v>
-      </c>
-      <c r="H10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10">
-        <v>0</v>
-      </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0</v>
-      </c>
-      <c r="G11" s="9">
-        <v>5.8</v>
-      </c>
-      <c r="H11" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>11</v>
-      </c>
-      <c r="B12" s="10">
-        <v>0</v>
-      </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7">
-        <v>0</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-      <c r="H12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>12</v>
-      </c>
-      <c r="B13" s="10">
-        <v>0</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7">
-        <v>0</v>
-      </c>
-      <c r="F13" s="7">
-        <v>0</v>
-      </c>
-      <c r="G13" s="9">
-        <v>11.2</v>
-      </c>
-      <c r="H13" s="9">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>13</v>
-      </c>
-      <c r="B14" s="10">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0</v>
-      </c>
-      <c r="H14" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>14</v>
-      </c>
-      <c r="B15" s="10">
-        <v>0</v>
-      </c>
-      <c r="C15" s="7">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7">
-        <v>0</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0</v>
-      </c>
-      <c r="G15" s="9">
-        <v>3.2</v>
-      </c>
-      <c r="H15" s="9">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>15</v>
-      </c>
-      <c r="B16" s="10">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0</v>
-      </c>
-      <c r="E16" s="7">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
-      <c r="G16" s="9">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="H16" s="9">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>16</v>
-      </c>
-      <c r="B17" s="10">
-        <v>0</v>
-      </c>
-      <c r="C17" s="7">
-        <v>1</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0</v>
-      </c>
-      <c r="E17" s="7">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7">
-        <v>0</v>
-      </c>
-      <c r="G17" s="9">
-        <v>3.5</v>
-      </c>
-      <c r="H17" s="9">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
-        <v>17</v>
-      </c>
-      <c r="B18" s="10">
-        <v>0</v>
-      </c>
-      <c r="C18" s="7">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7">
-        <v>0</v>
-      </c>
-      <c r="F18" s="7">
-        <v>0</v>
-      </c>
-      <c r="G18" s="11">
-        <v>9</v>
-      </c>
-      <c r="H18" s="11">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
-        <v>18</v>
-      </c>
-      <c r="B19" s="10">
-        <v>0</v>
-      </c>
-      <c r="C19" s="7">
-        <v>1</v>
-      </c>
-      <c r="D19" s="7">
-        <v>0</v>
-      </c>
-      <c r="E19" s="7">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="11">
-        <v>3.2</v>
-      </c>
-      <c r="H19" s="11">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
-        <v>19</v>
-      </c>
-      <c r="B20" s="10">
-        <v>0</v>
-      </c>
-      <c r="C20" s="7">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0</v>
-      </c>
-      <c r="G20" s="11">
-        <v>9.5</v>
-      </c>
-      <c r="H20" s="11">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="B21" s="10">
+        <v>0</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
+      <c r="G21" s="17">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H21" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="11">
         <v>20</v>
       </c>
-      <c r="B21" s="10">
-        <v>0</v>
-      </c>
-      <c r="C21" s="7">
-        <v>1</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7">
-        <v>0</v>
-      </c>
-      <c r="G21" s="11">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H21" s="11">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+      <c r="B22" s="10">
+        <v>0</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0</v>
+      </c>
+      <c r="G22" s="17">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="H22" s="17">
+        <v>0.112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
         <v>21</v>
       </c>
-      <c r="B22" s="10">
-        <v>0</v>
-      </c>
-      <c r="C22" s="7">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7">
-        <v>0</v>
-      </c>
-      <c r="E22" s="7">
-        <v>0</v>
-      </c>
-      <c r="F22" s="7">
-        <v>0</v>
-      </c>
-      <c r="G22" s="11">
-        <v>17.5</v>
-      </c>
-      <c r="H22" s="11">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="B23" s="10">
+        <v>0</v>
+      </c>
+      <c r="C23" s="7">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7">
+        <v>0</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0</v>
+      </c>
+      <c r="G23" s="17">
+        <v>0</v>
+      </c>
+      <c r="H23" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="11">
         <v>22</v>
       </c>
-      <c r="B23" s="10">
-        <v>0</v>
-      </c>
-      <c r="C23" s="7">
-        <v>1</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0</v>
-      </c>
-      <c r="E23" s="7">
-        <v>0</v>
-      </c>
-      <c r="F23" s="7">
-        <v>0</v>
-      </c>
-      <c r="G23" s="11">
-        <v>0</v>
-      </c>
-      <c r="H23" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+      <c r="B24" s="10">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0</v>
+      </c>
+      <c r="G24" s="17">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H24" s="17">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="11">
         <v>23</v>
       </c>
-      <c r="B24" s="10">
-        <v>0</v>
-      </c>
-      <c r="C24" s="7">
-        <v>1</v>
-      </c>
-      <c r="D24" s="7">
-        <v>0</v>
-      </c>
-      <c r="E24" s="7">
-        <v>0</v>
-      </c>
-      <c r="F24" s="7">
-        <v>0</v>
-      </c>
-      <c r="G24" s="11">
-        <v>3.2</v>
-      </c>
-      <c r="H24" s="11">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="B25" s="10">
+        <v>0</v>
+      </c>
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0</v>
+      </c>
+      <c r="G25" s="17">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="H25" s="17">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="11">
         <v>24</v>
       </c>
-      <c r="B25" s="10">
-        <v>0</v>
-      </c>
-      <c r="C25" s="7">
-        <v>1</v>
-      </c>
-      <c r="D25" s="7">
-        <v>0</v>
-      </c>
-      <c r="E25" s="7">
-        <v>0</v>
-      </c>
-      <c r="F25" s="7">
-        <v>0</v>
-      </c>
-      <c r="G25" s="11">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="H25" s="11">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="B26" s="10">
+        <v>0</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0</v>
+      </c>
+      <c r="G26" s="17">
+        <v>0</v>
+      </c>
+      <c r="H26" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
         <v>25</v>
       </c>
-      <c r="B26" s="10">
-        <v>0</v>
-      </c>
-      <c r="C26" s="7">
-        <v>1</v>
-      </c>
-      <c r="D26" s="7">
-        <v>0</v>
-      </c>
-      <c r="E26" s="7">
-        <v>0</v>
-      </c>
-      <c r="F26" s="7">
-        <v>0</v>
-      </c>
-      <c r="G26" s="11">
-        <v>0</v>
-      </c>
-      <c r="H26" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
+      <c r="B27" s="10">
+        <v>0</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0</v>
+      </c>
+      <c r="G27" s="17">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H27" s="17">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="11">
         <v>26</v>
       </c>
-      <c r="B27" s="10">
-        <v>0</v>
-      </c>
-      <c r="C27" s="7">
-        <v>1</v>
-      </c>
-      <c r="D27" s="7">
-        <v>0</v>
-      </c>
-      <c r="E27" s="7">
-        <v>0</v>
-      </c>
-      <c r="F27" s="7">
-        <v>0</v>
-      </c>
-      <c r="G27" s="11">
-        <v>3.5</v>
-      </c>
-      <c r="H27" s="11">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="B28" s="10">
+        <v>0</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0</v>
+      </c>
+      <c r="G28" s="17">
+        <v>0</v>
+      </c>
+      <c r="H28" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="11">
         <v>27</v>
       </c>
-      <c r="B28" s="10">
-        <v>0</v>
-      </c>
-      <c r="C28" s="7">
-        <v>1</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0</v>
-      </c>
-      <c r="E28" s="7">
-        <v>0</v>
-      </c>
-      <c r="F28" s="7">
-        <v>0</v>
-      </c>
-      <c r="G28" s="11">
-        <v>0</v>
-      </c>
-      <c r="H28" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
+      <c r="B29" s="10">
+        <v>0</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0</v>
+      </c>
+      <c r="G29" s="17">
+        <v>0</v>
+      </c>
+      <c r="H29" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="11">
         <v>28</v>
       </c>
-      <c r="B29" s="10">
-        <v>0</v>
-      </c>
-      <c r="C29" s="7">
-        <v>1</v>
-      </c>
-      <c r="D29" s="7">
-        <v>0</v>
-      </c>
-      <c r="E29" s="7">
-        <v>0</v>
-      </c>
-      <c r="F29" s="7">
-        <v>0</v>
-      </c>
-      <c r="G29" s="11">
-        <v>0</v>
-      </c>
-      <c r="H29" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+      <c r="B30" s="10">
+        <v>0</v>
+      </c>
+      <c r="C30" s="7">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0</v>
+      </c>
+      <c r="G30" s="17">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H30" s="17">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="11">
         <v>29</v>
       </c>
-      <c r="B30" s="10">
-        <v>0</v>
-      </c>
-      <c r="C30" s="7">
-        <v>1</v>
-      </c>
-      <c r="D30" s="7">
-        <v>0</v>
-      </c>
-      <c r="E30" s="7">
-        <v>0</v>
-      </c>
-      <c r="F30" s="7">
-        <v>0</v>
-      </c>
-      <c r="G30" s="11">
-        <v>2.4</v>
-      </c>
-      <c r="H30" s="11">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
-        <v>30</v>
-      </c>
       <c r="B31" s="10">
         <v>0</v>
       </c>
@@ -1312,11 +1332,11 @@
       <c r="F31" s="7">
         <v>0</v>
       </c>
-      <c r="G31" s="11">
-        <v>10.6</v>
-      </c>
-      <c r="H31" s="11">
-        <v>1.9</v>
+      <c r="G31" s="17">
+        <v>0.106</v>
+      </c>
+      <c r="H31" s="17">
+        <v>1.9E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1330,15 +1350,15 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1361,12 +1381,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="13">
         <v>1.9199999999999998E-2</v>
@@ -1384,12 +1404,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="13">
         <v>4.5199999999999997E-2</v>
@@ -1407,12 +1427,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="13">
         <v>5.7000000000000002E-2</v>
@@ -1430,12 +1450,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
         <v>3</v>
-      </c>
-      <c r="B5" s="6">
-        <v>4</v>
       </c>
       <c r="C5" s="13">
         <v>1.32E-2</v>
@@ -1453,12 +1473,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="13">
         <v>4.7199999999999999E-2</v>
@@ -1476,12 +1496,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="13">
         <v>5.8099999999999999E-2</v>
@@ -1499,12 +1519,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="13">
         <v>1.1900000000000001E-2</v>
@@ -1522,12 +1542,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="13">
         <v>4.5999999999999999E-2</v>
@@ -1545,12 +1565,12 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
         <v>6</v>
-      </c>
-      <c r="B10" s="1">
-        <v>7</v>
       </c>
       <c r="C10" s="13">
         <v>2.6700000000000002E-2</v>
@@ -1568,12 +1588,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="13">
         <v>1.2E-2</v>
@@ -1591,12 +1611,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="13">
         <v>0</v>
@@ -1614,12 +1634,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="13">
         <v>0</v>
@@ -1637,12 +1657,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="13">
         <v>0</v>
@@ -1660,12 +1680,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
+        <v>8</v>
+      </c>
+      <c r="B15" s="12">
         <v>9</v>
-      </c>
-      <c r="B15" s="12">
-        <v>10</v>
       </c>
       <c r="C15" s="14">
         <v>0</v>
@@ -1683,12 +1703,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="14">
         <v>0</v>
@@ -1706,12 +1726,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
+        <v>11</v>
+      </c>
+      <c r="B17" s="12">
         <v>12</v>
-      </c>
-      <c r="B17" s="12">
-        <v>13</v>
       </c>
       <c r="C17" s="14">
         <v>0</v>
@@ -1729,12 +1749,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="12">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="14">
         <v>0.1231</v>
@@ -1752,12 +1772,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="12">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="14">
         <v>6.6199999999999995E-2</v>
@@ -1775,12 +1795,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="12">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="14">
         <v>9.4500000000000001E-2</v>
@@ -1798,12 +1818,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
+        <v>13</v>
+      </c>
+      <c r="B21" s="12">
         <v>14</v>
-      </c>
-      <c r="B21" s="12">
-        <v>15</v>
       </c>
       <c r="C21" s="14">
         <v>0.221</v>
@@ -1821,12 +1841,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
+        <v>15</v>
+      </c>
+      <c r="B22" s="12">
         <v>16</v>
-      </c>
-      <c r="B22" s="12">
-        <v>17</v>
       </c>
       <c r="C22" s="14">
         <v>8.2400000000000001E-2</v>
@@ -1844,12 +1864,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="12">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="14">
         <v>0.107</v>
@@ -1867,12 +1887,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
+        <v>17</v>
+      </c>
+      <c r="B24" s="12">
         <v>18</v>
-      </c>
-      <c r="B24" s="12">
-        <v>19</v>
       </c>
       <c r="C24" s="14">
         <v>6.3899999999999998E-2</v>
@@ -1890,12 +1910,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
+        <v>18</v>
+      </c>
+      <c r="B25" s="12">
         <v>19</v>
-      </c>
-      <c r="B25" s="12">
-        <v>20</v>
       </c>
       <c r="C25" s="14">
         <v>3.4000000000000002E-2</v>
@@ -1913,12 +1933,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" s="12">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="14">
         <v>9.3600000000000003E-2</v>
@@ -1936,12 +1956,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="12">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="14">
         <v>3.2399999999999998E-2</v>
@@ -1959,12 +1979,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" s="12">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="14">
         <v>3.4799999999999998E-2</v>
@@ -1982,12 +2002,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" s="12">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" s="14">
         <v>7.2700000000000001E-2</v>
@@ -2005,12 +2025,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
+        <v>20</v>
+      </c>
+      <c r="B30" s="12">
         <v>21</v>
-      </c>
-      <c r="B30" s="12">
-        <v>22</v>
       </c>
       <c r="C30" s="14">
         <v>1.1599999999999999E-2</v>
@@ -2028,12 +2048,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="12">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" s="14">
         <v>0.1</v>
@@ -2051,12 +2071,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" s="12">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="14">
         <v>0.115</v>
@@ -2074,12 +2094,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
+        <v>22</v>
+      </c>
+      <c r="B33" s="12">
         <v>23</v>
-      </c>
-      <c r="B33" s="12">
-        <v>24</v>
       </c>
       <c r="C33" s="14">
         <v>0.13200000000000001</v>
@@ -2097,12 +2117,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
+        <v>23</v>
+      </c>
+      <c r="B34" s="12">
         <v>24</v>
-      </c>
-      <c r="B34" s="12">
-        <v>25</v>
       </c>
       <c r="C34" s="14">
         <v>0.1885</v>
@@ -2120,12 +2140,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
+        <v>24</v>
+      </c>
+      <c r="B35" s="12">
         <v>25</v>
-      </c>
-      <c r="B35" s="12">
-        <v>26</v>
       </c>
       <c r="C35" s="14">
         <v>0.25440000000000002</v>
@@ -2143,12 +2163,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="12">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" s="14">
         <v>0.10929999999999999</v>
@@ -2166,12 +2186,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="12">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C37" s="14">
         <v>0</v>
@@ -2189,12 +2209,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B38" s="12">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="14">
         <v>0.2198</v>
@@ -2212,12 +2232,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B39" s="12">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" s="14">
         <v>0.32019999999999998</v>
@@ -2235,12 +2255,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="12">
+        <v>28</v>
+      </c>
+      <c r="B40" s="12">
         <v>29</v>
-      </c>
-      <c r="B40" s="12">
-        <v>30</v>
       </c>
       <c r="C40" s="14">
         <v>0.2399</v>
@@ -2258,12 +2278,12 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41" s="12">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C41" s="14">
         <v>6.3600000000000004E-2</v>
@@ -2281,12 +2301,12 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42" s="12">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C42" s="14">
         <v>1.6899999999999998E-2</v>
@@ -2315,12 +2335,12 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -2346,163 +2366,163 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15">
         <v>8</v>
       </c>
-      <c r="D2" s="6">
-        <v>0</v>
+      <c r="D2" s="15">
+        <v>3.7499999999999999E-3</v>
       </c>
       <c r="E2" s="6">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="F2" s="6">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="G2" s="6">
         <v>0</v>
       </c>
       <c r="H2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15">
+        <v>12</v>
+      </c>
+      <c r="D3" s="15">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="G3" s="6">
+        <v>-0.2</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B4" s="15">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15">
         <v>12</v>
       </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>20</v>
-      </c>
-      <c r="F3" s="6">
-        <v>80</v>
-      </c>
-      <c r="G3" s="6">
-        <v>-20</v>
-      </c>
-      <c r="H3" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="D4" s="15">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="6">
+        <v>-0.15</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B5" s="15">
+        <v>0</v>
+      </c>
+      <c r="C5" s="15">
         <v>12</v>
       </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>15</v>
-      </c>
-      <c r="F4" s="6">
-        <v>50</v>
-      </c>
-      <c r="G4" s="6">
-        <v>-15</v>
-      </c>
-      <c r="H4" s="6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="D5" s="15">
+        <v>8.3400000000000002E-3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-0.15</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="B6" s="15">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15">
         <v>12</v>
       </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
-        <v>35</v>
-      </c>
-      <c r="G5" s="1">
-        <v>-15</v>
-      </c>
-      <c r="H5" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="D6" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-0.1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="B7" s="15">
+        <v>0</v>
+      </c>
+      <c r="C7" s="15">
         <v>12</v>
       </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1">
-        <v>30</v>
-      </c>
-      <c r="G6" s="1">
-        <v>-10</v>
-      </c>
-      <c r="H6" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>12</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
+      <c r="D7" s="15">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E7" s="1">
-        <v>12</v>
+        <v>0.12</v>
       </c>
       <c r="F7" s="1">
-        <v>40</v>
+        <v>0.4</v>
       </c>
       <c r="G7" s="1">
-        <v>-15</v>
+        <v>-0.15</v>
       </c>
       <c r="H7" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2512,7 +2532,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2522,7 +2542,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2532,7 +2552,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2542,7 +2562,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2552,7 +2572,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2562,7 +2582,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>

</xml_diff>